<commit_message>
Continued trying to set up an experiment by specifying information in spreadsheets, and interpreting using code. Created setup_functions.py to store the functions which perform this interpretation. Added my thoughts to notes.txt
</commit_message>
<xml_diff>
--- a/code-collab/database/chemical_inventory.xlsx
+++ b/code-collab/database/chemical_inventory.xlsx
@@ -10,7 +10,7 @@
   </mc:AlternateContent>
   <xr:revisionPtr revIDLastSave="0" documentId="8_{8F0300F4-BA5D-4CF3-96F6-480DF0FA8214}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1710" yWindow="-14370" windowWidth="14400" windowHeight="7365" xr2:uid="{8DB3FEF1-47EF-4BDE-A918-5C42E228C814}"/>
+    <workbookView xWindow="6810" yWindow="-9270" windowWidth="14400" windowHeight="7365" xr2:uid="{8DB3FEF1-47EF-4BDE-A918-5C42E228C814}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -519,7 +519,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{24B5398A-33C9-4627-B543-23FBE018D512}">
   <dimension ref="A1:O5"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="F6" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
       <selection activeCell="G12" activeCellId="1" sqref="K5 G12"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Minor changes to setup_functions and related excel/csv+notebook. Got vendor look-up working, needs to be transformed into module now.
</commit_message>
<xml_diff>
--- a/code-collab/database/chemical_inventory.xlsx
+++ b/code-collab/database/chemical_inventory.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://uwnetid-my.sharepoint.com/personal/lachok_uw_edu/Documents/Pozzo-RG-OT2/OT2Protocols/code-collab/database/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lacho\Documents\Pozzo-RG-OT2\OT2Protocols\code-collab\database\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{8F0300F4-BA5D-4CF3-96F6-480DF0FA8214}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5E8A8C95-88C1-4987-9F8C-ADADA4A8EBA2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6810" yWindow="-9270" windowWidth="14400" windowHeight="7365" xr2:uid="{8DB3FEF1-47EF-4BDE-A918-5C42E228C814}"/>
+    <workbookView xWindow="-120" yWindow="-16320" windowWidth="29040" windowHeight="15840" xr2:uid="{8DB3FEF1-47EF-4BDE-A918-5C42E228C814}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -519,8 +519,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{24B5398A-33C9-4627-B543-23FBE018D512}">
   <dimension ref="A1:O5"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F6" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="G12" activeCellId="1" sqref="K5 G12"/>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>

<commit_message>
Added log spacing as an option to setting up a lattice spacing experiment in the setup_functions.py and lattice_sampling csv
</commit_message>
<xml_diff>
--- a/code-collab/database/chemical_inventory.xlsx
+++ b/code-collab/database/chemical_inventory.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22624"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22730"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lacho\Documents\Pozzo-RG-OT2\OT2Protocols\code-collab\database\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5E8A8C95-88C1-4987-9F8C-ADADA4A8EBA2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{83399B40-8BA0-4A9A-AEA2-5BFD014E6B82}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-16320" windowWidth="29040" windowHeight="15840" xr2:uid="{8DB3FEF1-47EF-4BDE-A918-5C42E228C814}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{8DB3FEF1-47EF-4BDE-A918-5C42E228C814}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="48">
   <si>
     <t>Chemical Name</t>
   </si>
@@ -156,13 +156,34 @@
   </si>
   <si>
     <t>C5H14ClNO</t>
+  </si>
+  <si>
+    <t>haucl4</t>
+  </si>
+  <si>
+    <t>Gold (III) Chloride Trihydrate</t>
+  </si>
+  <si>
+    <t>1S/Au.4ClH.3H2O/h;4*1H;3*1H2/q+3;;;;;;;/p-3</t>
+  </si>
+  <si>
+    <t>XYYVDQWGDNRQDA-UHFFFAOYSA-K</t>
+  </si>
+  <si>
+    <t>AuCl4H7O3</t>
+  </si>
+  <si>
+    <t>O.O.O.Cl.Cl[Au](Cl)Cl</t>
+  </si>
+  <si>
+    <t>acid, inorganic</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -174,6 +195,12 @@
       <sz val="8"/>
       <color rgb="FF212121"/>
       <name val="Segoe UI"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <color rgb="FF222222"/>
+      <name val="Arial"/>
       <family val="2"/>
     </font>
   </fonts>
@@ -197,12 +224,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -517,9 +545,9 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{24B5398A-33C9-4627-B543-23FBE018D512}">
-  <dimension ref="A1:O5"/>
+  <dimension ref="A1:O6"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="130" workbookViewId="0">
       <selection activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>
@@ -529,7 +557,7 @@
     <col min="2" max="2" width="19.7265625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="22.453125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="13" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="6.26953125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="17.7265625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="12.26953125" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="16.26953125" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="20.6328125" bestFit="1" customWidth="1"/>
@@ -653,7 +681,7 @@
         <v>5234</v>
       </c>
     </row>
-    <row r="4" spans="1:15" ht="80.5" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:15" ht="34.5" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>27</v>
       </c>
@@ -685,7 +713,7 @@
         <v>723</v>
       </c>
     </row>
-    <row r="5" spans="1:15" ht="115" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:15" ht="34.5" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>34</v>
       </c>
@@ -712,6 +740,38 @@
       </c>
       <c r="J5">
         <v>6209</v>
+      </c>
+    </row>
+    <row r="6" spans="1:15" ht="34.5" x14ac:dyDescent="0.35">
+      <c r="A6" t="s">
+        <v>42</v>
+      </c>
+      <c r="B6" t="s">
+        <v>41</v>
+      </c>
+      <c r="C6" s="3">
+        <v>393.83</v>
+      </c>
+      <c r="D6">
+        <v>3.9</v>
+      </c>
+      <c r="E6" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="F6" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="G6" t="s">
+        <v>47</v>
+      </c>
+      <c r="H6" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="I6" t="s">
+        <v>45</v>
+      </c>
+      <c r="J6">
+        <v>44134746</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added excel sheet to handle solubility, and some code in a new notebook to show how it can be loaded in.
</commit_message>
<xml_diff>
--- a/code-collab/database/chemical_inventory.xlsx
+++ b/code-collab/database/chemical_inventory.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lacho\Documents\Pozzo-RG-OT2\OT2Protocols\code-collab\database\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{83399B40-8BA0-4A9A-AEA2-5BFD014E6B82}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{66B24761-46A1-4D98-9834-20876D763306}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{8DB3FEF1-47EF-4BDE-A918-5C42E228C814}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="1" xr2:uid="{8DB3FEF1-47EF-4BDE-A918-5C42E228C814}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Inventory" sheetId="1" r:id="rId1"/>
+    <sheet name="Solubility" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -33,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="56">
   <si>
     <t>Chemical Name</t>
   </si>
@@ -177,13 +178,37 @@
   </si>
   <si>
     <t>acid, inorganic</t>
+  </si>
+  <si>
+    <t>Component 1 Abbreviation</t>
+  </si>
+  <si>
+    <t>Solvent Abbreviation</t>
+  </si>
+  <si>
+    <t>Temperature °C</t>
+  </si>
+  <si>
+    <t>Component 1 Maximum g/L</t>
+  </si>
+  <si>
+    <t>Source</t>
+  </si>
+  <si>
+    <t>https://www.sigmaaldrich.com/content/dam/sigma-aldrich/docs/Sigma-Aldrich/Product_Information_Sheet/s7653pis.pdf</t>
+  </si>
+  <si>
+    <t>Yalkowsky, S.H., He, Yan, Jain, P. Handbook of Aqueous Solubility Data Second Edition. CRC Press, Boca Raton, FL 2010, p. 86</t>
+  </si>
+  <si>
+    <t>https://www.emdmillipore.com/US/en/product/TetrachloroauricIII-acid-trihydrate-990-0,MDA_CHEM-101582?ReferrerURL=https%3A%2F%2Fwww.google.com%2F&amp;bd=1</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -201,6 +226,21 @@
       <sz val="8"/>
       <color rgb="FF222222"/>
       <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="9.6"/>
+      <color rgb="FF5B616B"/>
+      <name val="Segoe UI"/>
       <family val="2"/>
     </font>
   </fonts>
@@ -221,18 +261,24 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -547,8 +593,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{24B5398A-33C9-4627-B543-23FBE018D512}">
   <dimension ref="A1:O6"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="D1" sqref="D1"/>
+    <sheetView topLeftCell="A2" zoomScale="80" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2:B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -778,4 +824,107 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C5575FA1-ABBE-4F01-8D63-F4C38DF4AB10}">
+  <dimension ref="A1:E5"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C6" sqref="C6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="2" width="23.08984375" customWidth="1"/>
+    <col min="3" max="3" width="23.453125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="23.08984375" customWidth="1"/>
+    <col min="5" max="5" width="104.54296875" bestFit="1" customWidth="1"/>
+    <col min="6" max="7" width="23.08984375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A1" t="s">
+        <v>48</v>
+      </c>
+      <c r="B1" t="s">
+        <v>49</v>
+      </c>
+      <c r="C1" t="s">
+        <v>51</v>
+      </c>
+      <c r="D1" t="s">
+        <v>50</v>
+      </c>
+      <c r="E1" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>22</v>
+      </c>
+      <c r="B2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C2">
+        <v>357</v>
+      </c>
+      <c r="D2">
+        <v>25</v>
+      </c>
+      <c r="E2" s="4" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>28</v>
+      </c>
+      <c r="B3" t="s">
+        <v>14</v>
+      </c>
+      <c r="C3">
+        <v>441</v>
+      </c>
+      <c r="D3">
+        <v>25</v>
+      </c>
+      <c r="E3" s="5" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
+        <v>35</v>
+      </c>
+      <c r="B4" t="s">
+        <v>14</v>
+      </c>
+      <c r="C4">
+        <v>650</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
+        <v>41</v>
+      </c>
+      <c r="B5" t="s">
+        <v>14</v>
+      </c>
+      <c r="C5">
+        <v>150</v>
+      </c>
+      <c r="E5" s="4" t="s">
+        <v>55</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="E2" r:id="rId1" xr:uid="{D938DB29-1BFF-49D1-B62F-2A759658EC96}"/>
+    <hyperlink ref="E5" r:id="rId2" xr:uid="{A54F0808-170D-491E-9EE3-B699F9A8EE05}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId3"/>
+</worksheet>
 </file>
</xml_diff>